<commit_message>
Enhanced coverage from 2026 not 2028
</commit_message>
<xml_diff>
--- a/sch_simulation/data/STH_params/ascaris_coverage_scenario_2.xlsx
+++ b/sch_simulation/data/STH_params/ascaris_coverage_scenario_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/GitHub/sch/ntd-model-sch/sch_simulation/data/STH_params/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2663F99-62F6-4B48-AEB2-93B581E75A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FE72FD-CB10-1A4D-9D36-FE9C2EBFABA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19160" xr2:uid="{2B23B0C0-4BFB-41FB-ACE5-EE30D4858695}"/>
   </bookViews>
@@ -450,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC57624-070C-4C6C-8EF3-3B0C0B08BDC6}">
   <dimension ref="A1:AD7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -587,7 +587,7 @@
         <v>0.6</v>
       </c>
       <c r="P2">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="R2">
         <v>0.8</v>
@@ -630,6 +630,9 @@
       <c r="G3">
         <v>50</v>
       </c>
+      <c r="P3">
+        <v>0.5</v>
+      </c>
       <c r="R3">
         <v>0.5</v>
       </c>
@@ -670,6 +673,9 @@
       </c>
       <c r="G4">
         <v>65</v>
+      </c>
+      <c r="P4">
+        <v>0.5</v>
       </c>
       <c r="R4">
         <v>0.5</v>
@@ -1014,12 +1020,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1240,15 +1243,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6338434B-B586-489B-A269-E3728BE15AC4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1273,10 +1280,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6338434B-B586-489B-A269-E3728BE15AC4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updating scenario file names (NOT FINAL VERSIONS)
</commit_message>
<xml_diff>
--- a/sch_simulation/data/STH_params/ascaris_coverage_scenario_2.xlsx
+++ b/sch_simulation/data/STH_params/ascaris_coverage_scenario_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/GitHub/sch/ntd-model-sch/sch_simulation/data/STH_params/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\ntd-model-sch\sch_simulation\data\STH_params\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FE72FD-CB10-1A4D-9D36-FE9C2EBFABA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F452AE4D-B71C-41A8-B397-480A7162CBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19160" xr2:uid="{2B23B0C0-4BFB-41FB-ACE5-EE30D4858695}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{2B23B0C0-4BFB-41FB-ACE5-EE30D4858695}"/>
   </bookViews>
   <sheets>
     <sheet name="Platform Coverage" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="20">
   <si>
     <t>Country/Region</t>
   </si>
@@ -448,22 +448,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC57624-070C-4C6C-8EF3-3B0C0B08BDC6}">
-  <dimension ref="A1:AD7"/>
+  <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="10.5" customWidth="1"/>
-    <col min="6" max="7" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -555,7 +555,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -569,7 +569,7 @@
         <v>3</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G2">
         <v>15</v>
@@ -586,32 +586,8 @@
       <c r="N2">
         <v>0.6</v>
       </c>
-      <c r="P2">
-        <v>0.8</v>
-      </c>
-      <c r="R2">
-        <v>0.8</v>
-      </c>
-      <c r="T2">
-        <v>0.8</v>
-      </c>
-      <c r="V2">
-        <v>0.8</v>
-      </c>
-      <c r="X2">
-        <v>0.8</v>
-      </c>
-      <c r="Z2">
-        <v>0.8</v>
-      </c>
-      <c r="AB2">
-        <v>0.8</v>
-      </c>
-      <c r="AD2">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -625,37 +601,37 @@
         <v>3</v>
       </c>
       <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
         <v>15</v>
       </c>
-      <c r="G3">
-        <v>50</v>
-      </c>
       <c r="P3">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="R3">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="T3">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="V3">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="X3">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="Z3">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="AB3">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="AD3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -669,11 +645,11 @@
         <v>3</v>
       </c>
       <c r="F4">
+        <v>15</v>
+      </c>
+      <c r="G4">
         <v>50</v>
       </c>
-      <c r="G4">
-        <v>65</v>
-      </c>
       <c r="P4">
         <v>0.5</v>
       </c>
@@ -699,27 +675,51 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
+      </c>
+      <c r="G5">
+        <v>65</v>
+      </c>
+      <c r="P5">
+        <v>0.5</v>
+      </c>
+      <c r="R5">
+        <v>0.5</v>
+      </c>
+      <c r="T5">
+        <v>0.5</v>
+      </c>
+      <c r="V5">
+        <v>0.5</v>
+      </c>
+      <c r="X5">
+        <v>0.5</v>
+      </c>
+      <c r="Z5">
+        <v>0.5</v>
+      </c>
+      <c r="AB5">
+        <v>0.5</v>
+      </c>
+      <c r="AD5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -730,16 +730,16 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -747,15 +747,35 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>15</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <v>100</v>
       </c>
     </row>
@@ -772,12 +792,12 @@
       <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -857,7 +877,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -868,7 +888,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -948,7 +968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -959,7 +979,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -970,7 +990,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -981,7 +1001,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -992,7 +1012,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1003,7 +1023,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1020,9 +1040,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1243,19 +1266,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6338434B-B586-489B-A269-E3728BE15AC4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1280,9 +1299,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6338434B-B586-489B-A269-E3728BE15AC4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
6 month coverage effective from 2026 for scenario 2
</commit_message>
<xml_diff>
--- a/sch_simulation/data/STH_params/ascaris_coverage_scenario_2.xlsx
+++ b/sch_simulation/data/STH_params/ascaris_coverage_scenario_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\ntd-model-sch\sch_simulation\data\STH_params\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F452AE4D-B71C-41A8-B397-480A7162CBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625D5AD3-8A9D-43CD-AC9A-3272410EC64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{2B23B0C0-4BFB-41FB-ACE5-EE30D4858695}"/>
   </bookViews>
@@ -448,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC57624-070C-4C6C-8EF3-3B0C0B08BDC6}">
-  <dimension ref="A1:AD8"/>
+  <dimension ref="A1:AZ8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AD2" sqref="AD2"/>
+      <selection activeCell="AW3" sqref="AW3:AW5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +463,7 @@
     <col min="6" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,73 +489,139 @@
         <v>2018</v>
       </c>
       <c r="I1">
+        <v>2018.5</v>
+      </c>
+      <c r="J1">
         <v>2019</v>
       </c>
-      <c r="J1">
+      <c r="K1">
+        <v>2019.5</v>
+      </c>
+      <c r="L1">
         <v>2020</v>
       </c>
-      <c r="K1">
+      <c r="M1">
+        <v>2020.5</v>
+      </c>
+      <c r="N1">
         <v>2021</v>
       </c>
-      <c r="L1">
+      <c r="O1">
+        <v>2021.5</v>
+      </c>
+      <c r="P1">
         <v>2022</v>
       </c>
-      <c r="M1">
+      <c r="Q1">
+        <v>2022.5</v>
+      </c>
+      <c r="R1">
         <v>2023</v>
       </c>
-      <c r="N1">
+      <c r="S1">
+        <v>2023.5</v>
+      </c>
+      <c r="T1">
         <v>2024</v>
       </c>
-      <c r="O1">
+      <c r="U1">
+        <v>2024.5</v>
+      </c>
+      <c r="V1">
         <v>2025</v>
       </c>
-      <c r="P1">
+      <c r="W1">
+        <v>2025.5</v>
+      </c>
+      <c r="X1">
         <v>2026</v>
       </c>
-      <c r="Q1">
+      <c r="Y1">
+        <v>2026.5</v>
+      </c>
+      <c r="Z1">
         <v>2027</v>
       </c>
-      <c r="R1">
+      <c r="AA1">
+        <v>2027.5</v>
+      </c>
+      <c r="AB1">
         <v>2028</v>
       </c>
-      <c r="S1">
+      <c r="AC1">
+        <v>2028.5</v>
+      </c>
+      <c r="AD1">
         <v>2029</v>
       </c>
-      <c r="T1">
+      <c r="AE1">
+        <v>2029.5</v>
+      </c>
+      <c r="AF1">
         <v>2030</v>
       </c>
-      <c r="U1">
+      <c r="AG1">
+        <v>2030.5</v>
+      </c>
+      <c r="AH1">
         <v>2031</v>
       </c>
-      <c r="V1">
+      <c r="AI1">
+        <v>2031.5</v>
+      </c>
+      <c r="AJ1">
         <v>2032</v>
       </c>
-      <c r="W1">
+      <c r="AK1">
+        <v>2032.5</v>
+      </c>
+      <c r="AL1">
         <v>2033</v>
       </c>
-      <c r="X1">
+      <c r="AM1">
+        <v>2033.5</v>
+      </c>
+      <c r="AN1">
         <v>2034</v>
       </c>
-      <c r="Y1">
+      <c r="AO1">
+        <v>2034.5</v>
+      </c>
+      <c r="AP1">
         <v>2035</v>
       </c>
-      <c r="Z1">
+      <c r="AQ1">
+        <v>2035.5</v>
+      </c>
+      <c r="AR1">
         <v>2036</v>
       </c>
-      <c r="AA1">
+      <c r="AS1">
+        <v>2036.5</v>
+      </c>
+      <c r="AT1">
         <v>2037</v>
       </c>
-      <c r="AB1">
+      <c r="AU1">
+        <v>2037.5</v>
+      </c>
+      <c r="AV1">
         <v>2038</v>
       </c>
-      <c r="AC1">
+      <c r="AW1">
+        <v>2038.5</v>
+      </c>
+      <c r="AX1">
         <v>2039</v>
       </c>
-      <c r="AD1">
+      <c r="AY1">
+        <v>2039.5</v>
+      </c>
+      <c r="AZ1">
         <v>2040</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -586,8 +652,20 @@
       <c r="N2">
         <v>0.6</v>
       </c>
+      <c r="P2">
+        <v>0.6</v>
+      </c>
+      <c r="R2">
+        <v>0.6</v>
+      </c>
+      <c r="T2">
+        <v>0.6</v>
+      </c>
+      <c r="V2">
+        <v>0.6</v>
+      </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -606,32 +684,95 @@
       <c r="G3">
         <v>15</v>
       </c>
-      <c r="P3">
-        <v>0.8</v>
-      </c>
-      <c r="R3">
-        <v>0.8</v>
-      </c>
-      <c r="T3">
-        <v>0.8</v>
-      </c>
-      <c r="V3">
-        <v>0.8</v>
-      </c>
       <c r="X3">
         <v>0.8</v>
       </c>
+      <c r="Y3">
+        <v>0.8</v>
+      </c>
       <c r="Z3">
         <v>0.8</v>
       </c>
+      <c r="AA3">
+        <v>0.8</v>
+      </c>
       <c r="AB3">
         <v>0.8</v>
       </c>
+      <c r="AC3">
+        <v>0.8</v>
+      </c>
       <c r="AD3">
         <v>0.8</v>
       </c>
+      <c r="AE3">
+        <v>0.8</v>
+      </c>
+      <c r="AF3">
+        <v>0.8</v>
+      </c>
+      <c r="AG3">
+        <v>0.8</v>
+      </c>
+      <c r="AH3">
+        <v>0.8</v>
+      </c>
+      <c r="AI3">
+        <v>0.8</v>
+      </c>
+      <c r="AJ3">
+        <v>0.8</v>
+      </c>
+      <c r="AK3">
+        <v>0.8</v>
+      </c>
+      <c r="AL3">
+        <v>0.8</v>
+      </c>
+      <c r="AM3">
+        <v>0.8</v>
+      </c>
+      <c r="AN3">
+        <v>0.8</v>
+      </c>
+      <c r="AO3">
+        <v>0.8</v>
+      </c>
+      <c r="AP3">
+        <v>0.8</v>
+      </c>
+      <c r="AQ3">
+        <v>0.8</v>
+      </c>
+      <c r="AR3">
+        <v>0.8</v>
+      </c>
+      <c r="AS3">
+        <v>0.8</v>
+      </c>
+      <c r="AT3">
+        <v>0.8</v>
+      </c>
+      <c r="AU3">
+        <v>0.8</v>
+      </c>
+      <c r="AV3">
+        <v>0.8</v>
+      </c>
+      <c r="AW3">
+        <v>0.8</v>
+      </c>
+      <c r="AX3">
+        <v>0.8</v>
+      </c>
+      <c r="AY3">
+        <v>0.8</v>
+      </c>
+      <c r="AZ3">
+        <v>0.8</v>
+      </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -650,32 +791,95 @@
       <c r="G4">
         <v>50</v>
       </c>
-      <c r="P4">
-        <v>0.5</v>
-      </c>
-      <c r="R4">
-        <v>0.5</v>
-      </c>
-      <c r="T4">
-        <v>0.5</v>
-      </c>
-      <c r="V4">
-        <v>0.5</v>
-      </c>
       <c r="X4">
         <v>0.5</v>
       </c>
+      <c r="Y4">
+        <v>0.5</v>
+      </c>
       <c r="Z4">
         <v>0.5</v>
       </c>
+      <c r="AA4">
+        <v>0.5</v>
+      </c>
       <c r="AB4">
         <v>0.5</v>
       </c>
+      <c r="AC4">
+        <v>0.5</v>
+      </c>
       <c r="AD4">
         <v>0.5</v>
       </c>
+      <c r="AE4">
+        <v>0.5</v>
+      </c>
+      <c r="AF4">
+        <v>0.5</v>
+      </c>
+      <c r="AG4">
+        <v>0.5</v>
+      </c>
+      <c r="AH4">
+        <v>0.5</v>
+      </c>
+      <c r="AI4">
+        <v>0.5</v>
+      </c>
+      <c r="AJ4">
+        <v>0.5</v>
+      </c>
+      <c r="AK4">
+        <v>0.5</v>
+      </c>
+      <c r="AL4">
+        <v>0.5</v>
+      </c>
+      <c r="AM4">
+        <v>0.5</v>
+      </c>
+      <c r="AN4">
+        <v>0.5</v>
+      </c>
+      <c r="AO4">
+        <v>0.5</v>
+      </c>
+      <c r="AP4">
+        <v>0.5</v>
+      </c>
+      <c r="AQ4">
+        <v>0.5</v>
+      </c>
+      <c r="AR4">
+        <v>0.5</v>
+      </c>
+      <c r="AS4">
+        <v>0.5</v>
+      </c>
+      <c r="AT4">
+        <v>0.5</v>
+      </c>
+      <c r="AU4">
+        <v>0.5</v>
+      </c>
+      <c r="AV4">
+        <v>0.5</v>
+      </c>
+      <c r="AW4">
+        <v>0.5</v>
+      </c>
+      <c r="AX4">
+        <v>0.5</v>
+      </c>
+      <c r="AY4">
+        <v>0.5</v>
+      </c>
+      <c r="AZ4">
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -694,32 +898,95 @@
       <c r="G5">
         <v>65</v>
       </c>
-      <c r="P5">
-        <v>0.5</v>
-      </c>
-      <c r="R5">
-        <v>0.5</v>
-      </c>
-      <c r="T5">
-        <v>0.5</v>
-      </c>
-      <c r="V5">
-        <v>0.5</v>
-      </c>
       <c r="X5">
         <v>0.5</v>
       </c>
+      <c r="Y5">
+        <v>0.5</v>
+      </c>
       <c r="Z5">
         <v>0.5</v>
       </c>
+      <c r="AA5">
+        <v>0.5</v>
+      </c>
       <c r="AB5">
         <v>0.5</v>
       </c>
+      <c r="AC5">
+        <v>0.5</v>
+      </c>
       <c r="AD5">
         <v>0.5</v>
       </c>
+      <c r="AE5">
+        <v>0.5</v>
+      </c>
+      <c r="AF5">
+        <v>0.5</v>
+      </c>
+      <c r="AG5">
+        <v>0.5</v>
+      </c>
+      <c r="AH5">
+        <v>0.5</v>
+      </c>
+      <c r="AI5">
+        <v>0.5</v>
+      </c>
+      <c r="AJ5">
+        <v>0.5</v>
+      </c>
+      <c r="AK5">
+        <v>0.5</v>
+      </c>
+      <c r="AL5">
+        <v>0.5</v>
+      </c>
+      <c r="AM5">
+        <v>0.5</v>
+      </c>
+      <c r="AN5">
+        <v>0.5</v>
+      </c>
+      <c r="AO5">
+        <v>0.5</v>
+      </c>
+      <c r="AP5">
+        <v>0.5</v>
+      </c>
+      <c r="AQ5">
+        <v>0.5</v>
+      </c>
+      <c r="AR5">
+        <v>0.5</v>
+      </c>
+      <c r="AS5">
+        <v>0.5</v>
+      </c>
+      <c r="AT5">
+        <v>0.5</v>
+      </c>
+      <c r="AU5">
+        <v>0.5</v>
+      </c>
+      <c r="AV5">
+        <v>0.5</v>
+      </c>
+      <c r="AW5">
+        <v>0.5</v>
+      </c>
+      <c r="AX5">
+        <v>0.5</v>
+      </c>
+      <c r="AY5">
+        <v>0.5</v>
+      </c>
+      <c r="AZ5">
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -739,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -759,7 +1026,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -786,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F794004A-4C7C-4E94-81C3-7E7CA0B5D399}">
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:AV9"/>
   <sheetViews>
-    <sheetView zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3"/>
+    <sheetView topLeftCell="AM1" zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:AV1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +1064,7 @@
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -811,73 +1078,139 @@
         <v>2018</v>
       </c>
       <c r="E1">
+        <v>2018.5</v>
+      </c>
+      <c r="F1">
         <v>2019</v>
       </c>
-      <c r="F1">
+      <c r="G1">
+        <v>2019.5</v>
+      </c>
+      <c r="H1">
         <v>2020</v>
       </c>
-      <c r="G1">
+      <c r="I1">
+        <v>2020.5</v>
+      </c>
+      <c r="J1">
         <v>2021</v>
       </c>
-      <c r="H1">
+      <c r="K1">
+        <v>2021.5</v>
+      </c>
+      <c r="L1">
         <v>2022</v>
       </c>
-      <c r="I1">
+      <c r="M1">
+        <v>2022.5</v>
+      </c>
+      <c r="N1">
         <v>2023</v>
       </c>
-      <c r="J1">
+      <c r="O1">
+        <v>2023.5</v>
+      </c>
+      <c r="P1">
         <v>2024</v>
       </c>
-      <c r="K1">
+      <c r="Q1">
+        <v>2024.5</v>
+      </c>
+      <c r="R1">
         <v>2025</v>
       </c>
-      <c r="L1">
+      <c r="S1">
+        <v>2025.5</v>
+      </c>
+      <c r="T1">
         <v>2026</v>
       </c>
-      <c r="M1">
+      <c r="U1">
+        <v>2026.5</v>
+      </c>
+      <c r="V1">
         <v>2027</v>
       </c>
-      <c r="N1">
+      <c r="W1">
+        <v>2027.5</v>
+      </c>
+      <c r="X1">
         <v>2028</v>
       </c>
-      <c r="O1">
+      <c r="Y1">
+        <v>2028.5</v>
+      </c>
+      <c r="Z1">
         <v>2029</v>
       </c>
-      <c r="P1">
+      <c r="AA1">
+        <v>2029.5</v>
+      </c>
+      <c r="AB1">
         <v>2030</v>
       </c>
-      <c r="Q1">
+      <c r="AC1">
+        <v>2030.5</v>
+      </c>
+      <c r="AD1">
         <v>2031</v>
       </c>
-      <c r="R1">
+      <c r="AE1">
+        <v>2031.5</v>
+      </c>
+      <c r="AF1">
         <v>2032</v>
       </c>
-      <c r="S1">
+      <c r="AG1">
+        <v>2032.5</v>
+      </c>
+      <c r="AH1">
         <v>2033</v>
       </c>
-      <c r="T1">
+      <c r="AI1">
+        <v>2033.5</v>
+      </c>
+      <c r="AJ1">
         <v>2034</v>
       </c>
-      <c r="U1">
+      <c r="AK1">
+        <v>2034.5</v>
+      </c>
+      <c r="AL1">
         <v>2035</v>
       </c>
-      <c r="V1">
+      <c r="AM1">
+        <v>2035.5</v>
+      </c>
+      <c r="AN1">
         <v>2036</v>
       </c>
-      <c r="W1">
+      <c r="AO1">
+        <v>2036.5</v>
+      </c>
+      <c r="AP1">
         <v>2037</v>
       </c>
-      <c r="X1">
+      <c r="AQ1">
+        <v>2037.5</v>
+      </c>
+      <c r="AR1">
         <v>2038</v>
       </c>
-      <c r="Y1">
+      <c r="AS1">
+        <v>2038.5</v>
+      </c>
+      <c r="AT1">
         <v>2039</v>
       </c>
-      <c r="Z1">
+      <c r="AU1">
+        <v>2039.5</v>
+      </c>
+      <c r="AV1">
         <v>2040</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -888,7 +1221,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -967,8 +1300,74 @@
       <c r="Z3">
         <v>1</v>
       </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+      <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AH3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <v>1</v>
+      </c>
+      <c r="AJ3">
+        <v>1</v>
+      </c>
+      <c r="AK3">
+        <v>1</v>
+      </c>
+      <c r="AL3">
+        <v>1</v>
+      </c>
+      <c r="AM3">
+        <v>1</v>
+      </c>
+      <c r="AN3">
+        <v>1</v>
+      </c>
+      <c r="AO3">
+        <v>1</v>
+      </c>
+      <c r="AP3">
+        <v>1</v>
+      </c>
+      <c r="AQ3">
+        <v>1</v>
+      </c>
+      <c r="AR3">
+        <v>1</v>
+      </c>
+      <c r="AS3">
+        <v>1</v>
+      </c>
+      <c r="AT3">
+        <v>1</v>
+      </c>
+      <c r="AU3">
+        <v>1</v>
+      </c>
+      <c r="AV3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -979,7 +1378,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -990,7 +1389,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1001,7 +1400,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1012,7 +1411,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1023,7 +1422,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1040,12 +1439,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1266,15 +1662,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6338434B-B586-489B-A269-E3728BE15AC4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1299,10 +1699,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6338434B-B586-489B-A269-E3728BE15AC4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>